<commit_message>
update hxl_example.xlsx fixture with correct version length
</commit_message>
<xml_diff>
--- a/onadata/apps/main/tests/fixtures/hxl_test/hxl_example.xlsx
+++ b/onadata/apps/main/tests/fixtures/hxl_test/hxl_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,37 +23,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>instance::hxl</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>#age</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>version</t>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instance::hxl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version</t>
   </si>
 </sst>
 </file>
@@ -61,9 +61,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -85,16 +85,139 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -102,8 +225,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -127,6 +265,54 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -134,14 +320,90 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -152,13 +414,13 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.4183673469388"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="13.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -203,7 +465,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -218,14 +480,14 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,13 +497,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>201604121155</v>
+        <v>2016041211</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>